<commit_message>
Begin with classification models
</commit_message>
<xml_diff>
--- a/OSA_CaseStudy/DATA/OSA_DB_cleaned.xlsx
+++ b/OSA_CaseStudy/DATA/OSA_DB_cleaned.xlsx
@@ -497,7 +497,7 @@
         <v>168</v>
       </c>
       <c r="G2" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H2" t="n">
         <v>29.05328798185942</v>
@@ -544,19 +544,19 @@
         <v>56</v>
       </c>
       <c r="D4" t="n">
-        <v>87.79703703703704</v>
+        <v>86</v>
       </c>
       <c r="E4" t="n">
         <v>46</v>
       </c>
       <c r="F4" t="n">
-        <v>171.3994082840237</v>
+        <v>171</v>
       </c>
       <c r="G4" t="n">
         <v>43</v>
       </c>
       <c r="H4" t="n">
-        <v>29.88554795334758</v>
+        <v>29.41075886597586</v>
       </c>
     </row>
     <row r="5">
@@ -777,7 +777,7 @@
         <v>182</v>
       </c>
       <c r="G12" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H12" t="n">
         <v>27.17063156623596</v>
@@ -805,7 +805,7 @@
         <v>169</v>
       </c>
       <c r="G13" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H13" t="n">
         <v>24.15881796855853</v>
@@ -2681,7 +2681,7 @@
         <v>175</v>
       </c>
       <c r="G80" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H80" t="n">
         <v>26.44897959183674</v>
@@ -5475,13 +5475,13 @@
         <v>106</v>
       </c>
       <c r="E180" t="n">
-        <v>49.50370370370371</v>
+        <v>49</v>
       </c>
       <c r="F180" t="n">
         <v>184</v>
       </c>
       <c r="G180" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H180" t="n">
         <v>31.30907372400756</v>
@@ -5503,13 +5503,13 @@
         <v>83</v>
       </c>
       <c r="E181" t="n">
-        <v>49.50370370370371</v>
+        <v>49</v>
       </c>
       <c r="F181" t="n">
         <v>175</v>
       </c>
       <c r="G181" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H181" t="n">
         <v>27.10204081632653</v>
@@ -5531,13 +5531,13 @@
         <v>71</v>
       </c>
       <c r="E182" t="n">
-        <v>49.50370370370371</v>
+        <v>49</v>
       </c>
       <c r="F182" t="n">
         <v>170</v>
       </c>
       <c r="G182" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H182" t="n">
         <v>24.56747404844291</v>
@@ -10988,19 +10988,19 @@
         <v>0</v>
       </c>
       <c r="D377" t="n">
-        <v>87.79703703703704</v>
+        <v>86</v>
       </c>
       <c r="E377" t="n">
         <v>71</v>
       </c>
       <c r="F377" t="n">
-        <v>171.3994082840237</v>
+        <v>171</v>
       </c>
       <c r="G377" t="n">
         <v>40</v>
       </c>
       <c r="H377" t="n">
-        <v>29.88554795334758</v>
+        <v>29.41075886597586</v>
       </c>
     </row>
     <row r="378">
@@ -15608,7 +15608,7 @@
         <v>5.3</v>
       </c>
       <c r="D542" t="n">
-        <v>87.79703703703704</v>
+        <v>86</v>
       </c>
       <c r="E542" t="n">
         <v>19</v>
@@ -15620,7 +15620,7 @@
         <v>39</v>
       </c>
       <c r="H542" t="n">
-        <v>31.48088387430064</v>
+        <v>30.83653053175087</v>
       </c>
     </row>
     <row r="543">
@@ -18044,19 +18044,19 @@
         <v>1.3</v>
       </c>
       <c r="D629" t="n">
-        <v>87.79703703703704</v>
+        <v>86</v>
       </c>
       <c r="E629" t="n">
-        <v>49.50370370370371</v>
+        <v>49</v>
       </c>
       <c r="F629" t="n">
-        <v>171.3994082840237</v>
+        <v>171</v>
       </c>
       <c r="G629" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H629" t="n">
-        <v>29.88554795334758</v>
+        <v>29.41075886597586</v>
       </c>
     </row>
     <row r="630">
@@ -18184,19 +18184,19 @@
         <v>1</v>
       </c>
       <c r="D634" t="n">
-        <v>87.79703703703704</v>
+        <v>86</v>
       </c>
       <c r="E634" t="n">
-        <v>49.50370370370371</v>
+        <v>49</v>
       </c>
       <c r="F634" t="n">
-        <v>171.3994082840237</v>
+        <v>171</v>
       </c>
       <c r="G634" t="n">
-        <v>40.6177347242921</v>
+        <v>41</v>
       </c>
       <c r="H634" t="n">
-        <v>29.88554795334758</v>
+        <v>29.41075886597586</v>
       </c>
     </row>
     <row r="635">

</xml_diff>